<commit_message>
rpi camera calibration done
</commit_message>
<xml_diff>
--- a/calibration-data/calibration.xlsx
+++ b/calibration-data/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Google Drive\Most Stuff\Documents\Current\EECS 149\project\ground-drone\calibration-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA365D7A-377C-4050-A268-143D54134F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB84EA1-AB28-44A0-8B39-B7233A430928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DDE4203E-6462-49BC-91F7-325AF51BDDE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>left steps</t>
   </si>
@@ -56,12 +56,6 @@
     <t>right distance/step</t>
   </si>
   <si>
-    <t>Pixel position</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
     <t>Pixel width</t>
   </si>
   <si>
@@ -69,6 +63,30 @@
   </si>
   <si>
     <t>Distance from ruler (mm)</t>
+  </si>
+  <si>
+    <t>Width of image (px)</t>
+  </si>
+  <si>
+    <t>measuring tape at center (mm)</t>
+  </si>
+  <si>
+    <t>pix</t>
+  </si>
+  <si>
+    <t>val (mm)</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>pix percent</t>
+  </si>
+  <si>
+    <t>opposite</t>
+  </si>
+  <si>
+    <t>adjacent</t>
   </si>
 </sst>
 </file>
@@ -121,6 +139,1034 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>angle</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs pixel percent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pixel Pos vs. Angle'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pix percent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pixel Pos vs. Angle'!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-29.810345265393014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-28.006247891865428</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-24.569489861370247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20.91644524980596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-17.130301526843592</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-13.127819249104283</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.8567148257320394</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.5037249955919032</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.4842236196015577</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0099042801069302</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.369505159409794</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.630684349771386</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.615098929044887</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.35967000187458</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28.976242395073893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.892363478300616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pixel Pos vs. Angle'!$H$2:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42BE-42D2-8893-DE113416B907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="533258400"/>
+        <c:axId val="533258816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="533258400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533258816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533258816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533258400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CE6F331-6B09-4673-8246-8EB83586F8BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,37 +1669,485 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756054A5-0592-4042-88C9-67CD4F9B92BD}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>292</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>777</v>
+      </c>
+      <c r="E2">
+        <f>D2-$A$6</f>
+        <v>-167.29999999999995</v>
+      </c>
+      <c r="F2">
+        <f>$A$2</f>
+        <v>292</v>
+      </c>
+      <c r="G2">
+        <f>ATAN(E2/F2)*180/PI()</f>
+        <v>-29.810345265393014</v>
+      </c>
+      <c r="H2">
+        <f>C2/$A$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>205</v>
+      </c>
+      <c r="D3">
+        <v>789</v>
+      </c>
+      <c r="E3">
+        <f>D3-$A$6</f>
+        <v>-155.29999999999995</v>
+      </c>
+      <c r="F3">
+        <f>$A$2</f>
+        <v>292</v>
+      </c>
+      <c r="G3">
+        <f>ATAN(E3/F3)*180/PI()</f>
+        <v>-28.006247891865428</v>
+      </c>
+      <c r="H3">
+        <f>C3/$A$4</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3280</v>
+      </c>
+      <c r="C4">
+        <f>C3+205</f>
+        <v>410</v>
+      </c>
+      <c r="D4">
+        <v>810.8</v>
+      </c>
+      <c r="E4">
+        <f>D4-$A$6</f>
+        <v>-133.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F18" si="0">$A$2</f>
+        <v>292</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G3:G18" si="1">ATAN(E4/F4)*180/PI()</f>
+        <v>-24.569489861370247</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H18" si="2">C4/$A$4</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>C4+205</f>
+        <v>615</v>
+      </c>
+      <c r="D5">
+        <v>832.7</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E4:E18" si="3">D5-$A$6</f>
+        <v>-111.59999999999991</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-20.91644524980596</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>944.3</v>
+      </c>
+      <c r="C6">
+        <f>C5+205</f>
+        <v>820</v>
+      </c>
+      <c r="D6">
+        <v>854.3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>-90</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-17.130301526843592</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>C6+205</f>
+        <v>1025</v>
+      </c>
+      <c r="D7">
+        <v>876.2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>-68.099999999999909</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-13.127819249104283</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f>C7+205</f>
+        <v>1230</v>
+      </c>
+      <c r="D8">
+        <v>898.8</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>-45.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-8.8567148257320394</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>C8+205</f>
+        <v>1435</v>
+      </c>
+      <c r="D9">
+        <v>921.3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>-23</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-4.5037249955919032</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>C9+205</f>
+        <v>1640</v>
+      </c>
+      <c r="D10">
+        <v>944.3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>C10+205</f>
+        <v>1845</v>
+      </c>
+      <c r="D11">
+        <v>967.2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>22.900000000000091</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>4.4842236196015577</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>C11+205</f>
+        <v>2050</v>
+      </c>
+      <c r="D12">
+        <v>990.6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>46.300000000000068</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>9.0099042801069302</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>C12+205</f>
+        <v>2255</v>
+      </c>
+      <c r="D13">
+        <v>1013.7</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>69.400000000000091</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>13.369505159409794</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>C13+205</f>
+        <v>2460</v>
+      </c>
+      <c r="D14">
+        <v>1037.0999999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>92.799999999999955</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>17.630684349771386</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>C14+205</f>
+        <v>2665</v>
+      </c>
+      <c r="D15">
+        <v>1060</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>115.70000000000005</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>21.615098929044887</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>C15+205</f>
+        <v>2870</v>
+      </c>
+      <c r="D16">
+        <v>1082.7</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>138.40000000000009</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>25.35967000187458</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>C16+205</f>
+        <v>3075</v>
+      </c>
+      <c r="D17">
+        <v>1106</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>161.70000000000005</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>28.976242395073893</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>C17+205</f>
+        <v>3280</v>
+      </c>
+      <c r="D18">
+        <v>1126</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>181.70000000000005</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="G18">
+        <f>ATAN(E18/F18)*180/PI()</f>
+        <v>31.892363478300616</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -669,10 +2163,10 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
website working on windows
</commit_message>
<xml_diff>
--- a/calibration-data/calibration.xlsx
+++ b/calibration-data/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Google Drive\Most Stuff\Documents\Current\EECS 149\project\ground-drone\calibration-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB84EA1-AB28-44A0-8B39-B7233A430928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC0532D-B261-4BBE-9EE6-652B1FFE3A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DDE4203E-6462-49BC-91F7-325AF51BDDE8}"/>
   </bookViews>
@@ -258,6 +258,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="#,##0.00000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Pixel Pos vs. Angle'!$G$2:$G$18</c:f>
@@ -572,7 +630,479 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>pixel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> percent vs angle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pixel Pos vs. Angle'!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>angle pix percent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pixel Pos vs. Angle'!$H$2:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pixel Pos vs. Angle'!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-29.810345265393014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-28.006247891865428</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-24.569489861370247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20.91644524980596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-17.130301526843592</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-13.127819249104283</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.8567148257320394</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.5037249955919032</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.4842236196015577</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0099042801069302</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.369505159409794</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.630684349771386</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.615098929044887</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.35967000187458</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28.976242395073893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.892363478300616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A411-4E52-90F8-14C6EB93D9E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1912796479"/>
+        <c:axId val="1912796895"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1912796479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1912796895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1912796895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1912796479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1128,20 +1658,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1161,6 +2207,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3DCD86-D62F-4DD7-9AE8-7F61AD4573F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1669,10 +2751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756054A5-0592-4042-88C9-67CD4F9B92BD}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +2766,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1707,7 +2789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>292</v>
       </c>
@@ -1733,8 +2815,12 @@
         <f>C2/$A$4</f>
         <v>0</v>
       </c>
+      <c r="I2">
+        <f>G2</f>
+        <v>-29.810345265393014</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1760,13 +2846,17 @@
         <f>C3/$A$4</f>
         <v>6.25E-2</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I18" si="0">G3</f>
+        <v>-28.006247891865428</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3280</v>
       </c>
       <c r="C4">
-        <f>C3+205</f>
+        <f t="shared" ref="C4:C18" si="1">C3+205</f>
         <v>410</v>
       </c>
       <c r="D4">
@@ -1777,363 +2867,419 @@
         <v>-133.5</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F18" si="0">$A$2</f>
+        <f t="shared" ref="F4:F18" si="2">$A$2</f>
         <v>292</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G3:G18" si="1">ATAN(E4/F4)*180/PI()</f>
+        <f t="shared" ref="G4:G17" si="3">ATAN(E4/F4)*180/PI()</f>
         <v>-24.569489861370247</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H18" si="2">C4/$A$4</f>
+        <f t="shared" ref="H4:H18" si="4">C4/$A$4</f>
         <v>0.125</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>-24.569489861370247</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <f>C4+205</f>
+        <f t="shared" si="1"/>
         <v>615</v>
       </c>
       <c r="D5">
         <v>832.7</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E4:E18" si="3">D5-$A$6</f>
+        <f t="shared" ref="E5:E18" si="5">D5-$A$6</f>
         <v>-111.59999999999991</v>
       </c>
       <c r="F5">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>-20.91644524980596</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>0.1875</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
         <v>-20.91644524980596</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
-        <v>0.1875</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>944.3</v>
       </c>
       <c r="C6">
-        <f>C5+205</f>
+        <f t="shared" si="1"/>
         <v>820</v>
       </c>
       <c r="D6">
         <v>854.3</v>
       </c>
       <c r="E6">
+        <f t="shared" si="5"/>
+        <v>-90</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="3"/>
-        <v>-90</v>
-      </c>
-      <c r="F6">
+        <v>-17.130301526843592</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G6">
+        <v>-17.130301526843592</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7">
         <f t="shared" si="1"/>
-        <v>-17.130301526843592</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <f>C6+205</f>
         <v>1025</v>
       </c>
       <c r="D7">
         <v>876.2</v>
       </c>
       <c r="E7">
+        <f t="shared" si="5"/>
+        <v>-68.099999999999909</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="3"/>
-        <v>-68.099999999999909</v>
-      </c>
-      <c r="F7">
+        <v>-13.127819249104283</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>0.3125</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G7">
+        <v>-13.127819249104283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8">
         <f t="shared" si="1"/>
-        <v>-13.127819249104283</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <f>C7+205</f>
         <v>1230</v>
       </c>
       <c r="D8">
         <v>898.8</v>
       </c>
       <c r="E8">
+        <f t="shared" si="5"/>
+        <v>-45.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="3"/>
-        <v>-45.5</v>
-      </c>
-      <c r="F8">
+        <v>-8.8567148257320394</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G8">
+        <v>-8.8567148257320394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9">
         <f t="shared" si="1"/>
-        <v>-8.8567148257320394</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <f>C8+205</f>
         <v>1435</v>
       </c>
       <c r="D9">
         <v>921.3</v>
       </c>
       <c r="E9">
+        <f t="shared" si="5"/>
+        <v>-23</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="3"/>
-        <v>-23</v>
-      </c>
-      <c r="F9">
+        <v>-4.5037249955919032</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0.4375</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G9">
+        <v>-4.5037249955919032</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10">
         <f t="shared" si="1"/>
-        <v>-4.5037249955919032</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <f>C9+205</f>
         <v>1640</v>
       </c>
       <c r="D10">
         <v>944.3</v>
       </c>
       <c r="E10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f>C10+205</f>
         <v>1845</v>
       </c>
       <c r="D11">
         <v>967.2</v>
       </c>
       <c r="E11">
+        <f t="shared" si="5"/>
+        <v>22.900000000000091</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="3"/>
-        <v>22.900000000000091</v>
-      </c>
-      <c r="F11">
+        <v>4.4842236196015577</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>0.5625</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G11">
+        <v>4.4842236196015577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12">
         <f t="shared" si="1"/>
-        <v>4.4842236196015577</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <f>C11+205</f>
         <v>2050</v>
       </c>
       <c r="D12">
         <v>990.6</v>
       </c>
       <c r="E12">
+        <f t="shared" si="5"/>
+        <v>46.300000000000068</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="3"/>
-        <v>46.300000000000068</v>
-      </c>
-      <c r="F12">
+        <v>9.0099042801069302</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G12">
+        <v>9.0099042801069302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13">
         <f t="shared" si="1"/>
-        <v>9.0099042801069302</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f>C12+205</f>
         <v>2255</v>
       </c>
       <c r="D13">
         <v>1013.7</v>
       </c>
       <c r="E13">
+        <f t="shared" si="5"/>
+        <v>69.400000000000091</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="3"/>
-        <v>69.400000000000091</v>
-      </c>
-      <c r="F13">
+        <v>13.369505159409794</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>0.6875</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G13">
+        <v>13.369505159409794</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14">
         <f t="shared" si="1"/>
-        <v>13.369505159409794</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <f>C13+205</f>
         <v>2460</v>
       </c>
       <c r="D14">
         <v>1037.0999999999999</v>
       </c>
       <c r="E14">
+        <f t="shared" si="5"/>
+        <v>92.799999999999955</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="3"/>
-        <v>92.799999999999955</v>
-      </c>
-      <c r="F14">
+        <v>17.630684349771386</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G14">
+        <v>17.630684349771386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15">
         <f t="shared" si="1"/>
-        <v>17.630684349771386</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f>C14+205</f>
         <v>2665</v>
       </c>
       <c r="D15">
         <v>1060</v>
       </c>
       <c r="E15">
+        <f t="shared" si="5"/>
+        <v>115.70000000000005</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="3"/>
-        <v>115.70000000000005</v>
-      </c>
-      <c r="F15">
+        <v>21.615098929044887</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>0.8125</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G15">
+        <v>21.615098929044887</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16">
         <f t="shared" si="1"/>
-        <v>21.615098929044887</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <f>C15+205</f>
         <v>2870</v>
       </c>
       <c r="D16">
         <v>1082.7</v>
       </c>
       <c r="E16">
+        <f t="shared" si="5"/>
+        <v>138.40000000000009</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="3"/>
-        <v>138.40000000000009</v>
-      </c>
-      <c r="F16">
+        <v>25.35967000187458</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>0.875</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G16">
+        <v>25.35967000187458</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17">
         <f t="shared" si="1"/>
-        <v>25.35967000187458</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <f>C16+205</f>
         <v>3075</v>
       </c>
       <c r="D17">
         <v>1106</v>
       </c>
       <c r="E17">
+        <f t="shared" si="5"/>
+        <v>161.70000000000005</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="3"/>
-        <v>161.70000000000005</v>
-      </c>
-      <c r="F17">
+        <v>28.976242395073893</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>0.9375</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="0"/>
-        <v>292</v>
-      </c>
-      <c r="G17">
+        <v>28.976242395073893</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18">
         <f t="shared" si="1"/>
-        <v>28.976242395073893</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <f>C17+205</f>
         <v>3280</v>
       </c>
       <c r="D18">
         <v>1126</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>181.70000000000005</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
       <c r="G18">
@@ -2141,8 +3287,12 @@
         <v>31.892363478300616</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>31.892363478300616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>